<commit_message>
update one more test case
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/validation/cases/stochastic/00021/00021-wc_lang.xlsx
+++ b/tests/multialgorithm/fixtures/validation/cases/stochastic/00021/00021-wc_lang.xlsx
@@ -400,9 +400,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
@@ -437,9 +438,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>

</xml_diff>